<commit_message>
updated commit code size spreadsheets
</commit_message>
<xml_diff>
--- a/xlsx/Commits_Code_Size.xlsx
+++ b/xlsx/Commits_Code_Size.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dylan\Documents\Computer Science Projects\miningMatplotlib\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dylan\PycharmProjects\miningMatplotlib\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F1BBCD2-0993-47B1-ACF4-95200AC61845}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABF5BA60-8E3B-41BD-9532-4FC75E72FB5B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2196" yWindow="2196" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>Commits Timeline</t>
   </si>
@@ -51,7 +51,10 @@
     <t>Last 1K Commits</t>
   </si>
   <si>
-    <t>Percentage Increase From Baseline to Selected Commit Timeline</t>
+    <t>Average Source Files Per Commit Timeline</t>
+  </si>
+  <si>
+    <t>Percentage From Timeline Selected Commit Timeline</t>
   </si>
 </sst>
 </file>
@@ -274,13 +277,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>5076913.9620000003</c:v>
+                  <c:v>445918.21600000001</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>83568167.363999993</c:v>
+                  <c:v>6095756.0530000003</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>68142661.991999999</c:v>
+                  <c:v>3733179.9980000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -625,7 +628,7 @@
     <c:plotArea>
       <c:layout/>
       <c:barChart>
-        <c:barDir val="bar"/>
+        <c:barDir val="col"/>
         <c:grouping val="clustered"/>
         <c:varyColors val="0"/>
         <c:ser>
@@ -633,14 +636,11 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$C$1:$C$2</c:f>
+              <c:f>Sheet1!$C$1</c:f>
               <c:strCache>
-                <c:ptCount val="2"/>
+                <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Percentage Increase From Baseline to Selected Commit Timeline</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>Average Source Files Per Commit Timeline</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -657,13 +657,16 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$3:$A$4</c:f>
+              <c:f>Sheet1!$A$2:$A$4</c:f>
               <c:strCache>
-                <c:ptCount val="2"/>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
+                  <c:v>First 1K Commits</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>Middle Thousand Commits</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>Last 1K Commits</c:v>
                 </c:pt>
               </c:strCache>
@@ -671,22 +674,25 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$C$3:$C$4</c:f>
+              <c:f>Sheet1!$C$2:$C$4</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="2"/>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>15.460426154450555</c:v>
+                  <c:v>30.39</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>13.422063580757603</c:v>
+                  <c:v>330.92500000000001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>300.63600000000002</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-E8A2-41A7-A744-E7BDF02B5320}"/>
+              <c16:uniqueId val="{00000000-1D67-4A2B-A6E8-EE64C0629A4D}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -698,17 +704,18 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:gapWidth val="182"/>
-        <c:axId val="408588528"/>
-        <c:axId val="408573552"/>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="501467128"/>
+        <c:axId val="501471064"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="408588528"/>
+        <c:axId val="501467128"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
-        <c:axPos val="l"/>
+        <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -746,7 +753,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="408573552"/>
+        <c:crossAx val="501471064"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -754,12 +761,12 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="408573552"/>
+        <c:axId val="501471064"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
-        <c:axPos val="b"/>
+        <c:axPos val="l"/>
         <c:majorGridlines>
           <c:spPr>
             <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
@@ -805,7 +812,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="408588528"/>
+        <c:crossAx val="501467128"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -819,6 +826,13 @@
     </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
     <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
@@ -1438,7 +1452,7 @@
 </file>
 
 <file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="216">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
@@ -1642,23 +1656,22 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="dk1">
-          <a:lumMod val="75000"/>
-          <a:lumOff val="25000"/>
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
         </a:schemeClr>
       </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="tx1">
             <a:lumMod val="65000"/>
             <a:lumOff val="35000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:downBar>
@@ -1763,8 +1776,8 @@
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="50000"/>
-            <a:lumOff val="50000"/>
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -1896,20 +1909,19 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="lt1"/>
       </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
       </a:ln>
     </cs:spPr>
   </cs:upBar>
@@ -1983,22 +1995,22 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>2314575</xdr:colOff>
+      <xdr:colOff>2377440</xdr:colOff>
       <xdr:row>5</xdr:row>
-      <xdr:rowOff>14287</xdr:rowOff>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>361950</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>90487</xdr:rowOff>
+      <xdr:colOff>342900</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Chart 2">
+        <xdr:cNvPr id="4" name="Chart 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{367344E8-DAF1-4E7C-9D3F-A22857ADD0D2}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{63874A8E-A8FF-4A36-A68F-BF5ECA98AB94}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2282,20 +2294,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="33.77734375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="43" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2305,40 +2317,41 @@
       <c r="C1" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="D1" s="1" t="s">
+        <v>6</v>
+      </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>2</v>
       </c>
       <c r="B2">
-        <v>5076913.9620000003</v>
+        <v>445918.21600000001</v>
       </c>
-      <c r="C2" s="1">
-        <v>0</v>
+      <c r="C2">
+        <v>30.39</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>1</v>
       </c>
       <c r="B3">
-        <v>83568167.363999993</v>
+        <v>6095756.0530000003</v>
       </c>
       <c r="C3" s="2">
-        <f>((B3/B2) - 1)</f>
-        <v>15.460426154450555</v>
+        <v>330.92500000000001</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>4</v>
       </c>
       <c r="B4">
-        <v>68142661.991999999</v>
+        <v>3733179.9980000001</v>
       </c>
       <c r="C4" s="1">
-        <f>(B4/B2)</f>
-        <v>13.422063580757603</v>
+        <v>300.63600000000002</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added issue density excel file
</commit_message>
<xml_diff>
--- a/xlsx/Commits_Code_Size.xlsx
+++ b/xlsx/Commits_Code_Size.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dylan\PycharmProjects\miningMatplotlib\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABF5BA60-8E3B-41BD-9532-4FC75E72FB5B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62D5963F-15FE-437A-9C57-4C94C1CAA278}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2196" yWindow="2196" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1152" yWindow="1152" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -51,10 +51,10 @@
     <t>Last 1K Commits</t>
   </si>
   <si>
-    <t>Average Source Files Per Commit Timeline</t>
+    <t>Percentage From Timeline Selected Commit Timeline</t>
   </si>
   <si>
-    <t>Percentage From Timeline Selected Commit Timeline</t>
+    <t>Average Source Files Count Per Commit Timeline</t>
   </si>
 </sst>
 </file>
@@ -640,7 +640,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Average Source Files Per Commit Timeline</c:v>
+                  <c:v>Average Source Files Count Per Commit Timeline</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -655,6 +655,64 @@
             <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
           <c:cat>
             <c:strRef>
               <c:f>Sheet1!$A$2:$A$4</c:f>
@@ -697,8 +755,9 @@
           </c:extLst>
         </c:ser>
         <c:dLbls>
+          <c:dLblPos val="outEnd"/>
           <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
+          <c:showVal val="1"/>
           <c:showCatName val="0"/>
           <c:showSerName val="0"/>
           <c:showPercent val="0"/>
@@ -716,6 +775,66 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Commit</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> Timeline</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -781,6 +900,66 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>#</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> Source Files</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -2296,8 +2475,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" topLeftCell="C5" workbookViewId="0">
+      <selection activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2315,10 +2494,10 @@
         <v>3</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">

</xml_diff>